<commit_message>
calibration and test changes
calibration adjustment, analysis, correcting_interface, ping test, rps changes
</commit_message>
<xml_diff>
--- a/BLE_connect_and_control_script/2021_11_17_16_11_46_1.xlsx
+++ b/BLE_connect_and_control_script/2021_11_17_16_11_46_1.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasornstein/Documents/CSBABY/fulbright_projects/openEMSstim/BLE_connect_and_control_script/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6E73D9-0673-A843-A424-C5997B326205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pain level" sheetId="1" r:id="rId1"/>
     <sheet name="Actuation level" sheetId="2" r:id="rId2"/>
     <sheet name="Actuation speed" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -72,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +125,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -165,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +211,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,6 +263,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,14 +456,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -471,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -494,7 +546,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20</v>
       </c>
@@ -517,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>30</v>
       </c>
@@ -540,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -563,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50</v>
       </c>
@@ -586,7 +638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>60</v>
       </c>
@@ -609,7 +661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>70</v>
       </c>
@@ -632,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>80</v>
       </c>
@@ -646,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -655,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>90</v>
       </c>
@@ -684,14 +736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,7 +772,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -749,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -772,7 +824,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20</v>
       </c>
@@ -795,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>30</v>
       </c>
@@ -818,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -841,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50</v>
       </c>
@@ -864,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>60</v>
       </c>
@@ -887,7 +939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>70</v>
       </c>
@@ -910,7 +962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>80</v>
       </c>
@@ -933,7 +985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>90</v>
       </c>
@@ -962,14 +1014,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1050,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1027,7 +1079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1050,7 +1102,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20</v>
       </c>
@@ -1073,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>30</v>
       </c>
@@ -1096,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1119,7 +1171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50</v>
       </c>
@@ -1142,7 +1194,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>60</v>
       </c>
@@ -1165,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>70</v>
       </c>
@@ -1188,7 +1240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>80</v>
       </c>
@@ -1211,7 +1263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>90</v>
       </c>

</xml_diff>